<commit_message>
Creates a class 'DictReader' to handle data dictionary validation and conversion to an autoparser-usable format. Builds that into existing code and allows current example script to still run.
</commit_message>
<xml_diff>
--- a/tests/test_autoparser/sources/animal_data.xlsx
+++ b/tests/test_autoparser/sources/animal_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pipliggins/Documents/repos/autoparser/tests/sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pipliggins/Documents/repos/adtl/tests/test_autoparser/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D4FEC8-53B9-D74F-9DF7-6289071C5618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C27901-2CB8-AE48-AFD4-2CA95FF4337F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{15744167-E704-8C46-A2E1-4C8DCF4B5253}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>ContHumain Autre</t>
   </si>
   <si>
-    <t>AutreContHumain</t>
-  </si>
-  <si>
     <t>ContactAnimal</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>Mammifère</t>
+  </si>
+  <si>
+    <t>ContexteContHumain</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -821,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1200,14 +1200,14 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1246,33 +1246,33 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="3">
         <v>45292</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1">
         <v>44635</v>
@@ -1284,45 +1284,45 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="1">
         <v>44398</v>
@@ -1334,48 +1334,48 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K3" s="1">
         <v>45444</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
       <c r="Q3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
         <v>45361</v>
       </c>
       <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
       </c>
       <c r="F4" s="1">
         <v>44967</v>
@@ -1387,42 +1387,42 @@
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3">
         <v>45404</v>
       </c>
       <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
         <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
       </c>
       <c r="F5" s="1">
         <v>44140</v>
@@ -1434,39 +1434,39 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
         <v>45442</v>
       </c>
       <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
       </c>
       <c r="F6" s="1">
         <v>43603</v>
@@ -1478,39 +1478,39 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K6" s="1">
         <v>45474</v>
       </c>
       <c r="N6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3">
         <v>45296</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="1">
         <v>44630</v>
@@ -1522,42 +1522,42 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3">
         <v>45458</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1">
         <v>44368</v>
@@ -1569,45 +1569,45 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K8" s="1">
         <v>45473</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3">
         <v>45483</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1">
         <v>44602</v>
@@ -1619,45 +1619,45 @@
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
       </c>
       <c r="C10" s="3">
         <v>45392</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="1">
         <v>44142</v>
@@ -1669,42 +1669,42 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3">
         <v>45290</v>
       </c>
       <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>53</v>
       </c>
       <c r="F11" s="1">
         <v>45064</v>
@@ -1716,48 +1716,48 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K11" s="1">
         <v>45306</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3">
         <v>44562</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1">
         <v>43174</v>
@@ -1769,42 +1769,42 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3">
         <v>44972</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1">
         <v>44276</v>
@@ -1816,42 +1816,42 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K13" s="1">
         <v>45448</v>
       </c>
       <c r="N13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" t="s">
         <v>27</v>
       </c>
-      <c r="O13" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13" t="s">
-        <v>28</v>
-      </c>
       <c r="Q13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
       </c>
       <c r="C14" s="3">
         <v>43900</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1">
         <v>45240</v>
@@ -1863,39 +1863,39 @@
         <v>11</v>
       </c>
       <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" t="s">
         <v>62</v>
-      </c>
-      <c r="J14" t="s">
-        <v>19</v>
-      </c>
-      <c r="N14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="3">
         <v>44308</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1">
         <v>44148</v>
@@ -1907,39 +1907,39 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3">
         <v>45443</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="1">
         <v>43586</v>
@@ -1951,48 +1951,48 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K16" s="1">
         <v>45488</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>45299</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="1">
         <v>44628</v>
@@ -2004,45 +2004,45 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
         <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
       </c>
       <c r="C18" s="3">
         <v>45347</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1">
         <v>44307</v>
@@ -2054,48 +2054,48 @@
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K18" s="1">
         <v>45444</v>
       </c>
       <c r="L18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3">
         <v>45453</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1">
         <v>45061</v>
@@ -2107,45 +2107,45 @@
         <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3">
         <v>45618</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="1">
         <v>44048</v>
@@ -2157,45 +2157,45 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="1">
         <v>43660</v>
@@ -2207,45 +2207,45 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K21" s="1">
         <v>45366</v>
       </c>
       <c r="M21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3">
         <v>45364</v>
       </c>
       <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
         <v>30</v>
-      </c>
-      <c r="E22" t="s">
-        <v>31</v>
       </c>
       <c r="F22" s="1">
         <v>44939</v>
@@ -2257,39 +2257,39 @@
         <v>11</v>
       </c>
       <c r="I22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="3">
         <v>45399</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="1">
         <v>44113</v>
@@ -2301,36 +2301,36 @@
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="3">
         <v>45432</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" s="1">
         <v>43613</v>
@@ -2342,42 +2342,42 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K24" s="1">
         <v>45454</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3">
         <v>45597</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="1">
         <v>44755</v>
@@ -2389,42 +2389,42 @@
         <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="3">
         <v>45327</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F26" s="1">
         <v>44388</v>
@@ -2436,45 +2436,45 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K26" s="1">
         <v>45352</v>
       </c>
       <c r="L26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N26" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" t="s">
+        <v>20</v>
+      </c>
+      <c r="P26" t="s">
         <v>27</v>
       </c>
-      <c r="O26" t="s">
-        <v>21</v>
-      </c>
-      <c r="P26" t="s">
-        <v>28</v>
-      </c>
       <c r="Q26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="3">
         <v>45636</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" s="1">
         <v>44995</v>
@@ -2486,42 +2486,42 @@
         <v>11</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="3">
         <v>45411</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F28" s="1">
         <v>43044</v>
@@ -2533,42 +2533,42 @@
         <v>5</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" s="3">
         <v>45565</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F29" s="1">
         <v>43817</v>
@@ -2580,42 +2580,42 @@
         <v>3</v>
       </c>
       <c r="I29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K29" s="1">
         <v>45412</v>
       </c>
       <c r="L29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="3">
         <v>45323</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="1">
         <v>44633</v>
@@ -2627,45 +2627,45 @@
         <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="3">
         <v>45334</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F31" s="1">
         <v>44551</v>
@@ -2677,31 +2677,31 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K31" s="1">
         <v>45347</v>
       </c>
       <c r="L31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N31" t="s">
+        <v>26</v>
+      </c>
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+      <c r="P31" t="s">
         <v>27</v>
       </c>
-      <c r="O31" t="s">
-        <v>21</v>
-      </c>
-      <c r="P31" t="s">
-        <v>28</v>
-      </c>
       <c r="Q31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add outside data dictionary (#138)
* Allow a data dictionary to be supplied with potential duplicate descriptions.

* use pandas[parquet] for parquet, not polars

* Creates a class 'DictReader' to handle data dictionary validation and conversion to an autoparser-usable format.
Builds that into existing code and allows current example script to still run.

* Keep boolean True/False values in data dict even though not strings

* Increase version now new functionality is present
</commit_message>
<xml_diff>
--- a/tests/test_autoparser/sources/animal_data.xlsx
+++ b/tests/test_autoparser/sources/animal_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pipliggins/Documents/repos/autoparser/tests/sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pipliggins/Documents/repos/adtl/tests/test_autoparser/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D4FEC8-53B9-D74F-9DF7-6289071C5618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C27901-2CB8-AE48-AFD4-2CA95FF4337F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{15744167-E704-8C46-A2E1-4C8DCF4B5253}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>ContHumain Autre</t>
   </si>
   <si>
-    <t>AutreContHumain</t>
-  </si>
-  <si>
     <t>ContactAnimal</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>Mammifère</t>
+  </si>
+  <si>
+    <t>ContexteContHumain</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -821,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1200,14 +1200,14 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1246,33 +1246,33 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="3">
         <v>45292</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1">
         <v>44635</v>
@@ -1284,45 +1284,45 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="1">
         <v>44398</v>
@@ -1334,48 +1334,48 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K3" s="1">
         <v>45444</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="O3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
       <c r="Q3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
         <v>45361</v>
       </c>
       <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
       </c>
       <c r="F4" s="1">
         <v>44967</v>
@@ -1387,42 +1387,42 @@
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3">
         <v>45404</v>
       </c>
       <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
         <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
       </c>
       <c r="F5" s="1">
         <v>44140</v>
@@ -1434,39 +1434,39 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
         <v>45442</v>
       </c>
       <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
       </c>
       <c r="F6" s="1">
         <v>43603</v>
@@ -1478,39 +1478,39 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K6" s="1">
         <v>45474</v>
       </c>
       <c r="N6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3">
         <v>45296</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="1">
         <v>44630</v>
@@ -1522,42 +1522,42 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3">
         <v>45458</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1">
         <v>44368</v>
@@ -1569,45 +1569,45 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K8" s="1">
         <v>45473</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3">
         <v>45483</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1">
         <v>44602</v>
@@ -1619,45 +1619,45 @@
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
       </c>
       <c r="C10" s="3">
         <v>45392</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="1">
         <v>44142</v>
@@ -1669,42 +1669,42 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3">
         <v>45290</v>
       </c>
       <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>53</v>
       </c>
       <c r="F11" s="1">
         <v>45064</v>
@@ -1716,48 +1716,48 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K11" s="1">
         <v>45306</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3">
         <v>44562</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1">
         <v>43174</v>
@@ -1769,42 +1769,42 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3">
         <v>44972</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1">
         <v>44276</v>
@@ -1816,42 +1816,42 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K13" s="1">
         <v>45448</v>
       </c>
       <c r="N13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" t="s">
         <v>27</v>
       </c>
-      <c r="O13" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13" t="s">
-        <v>28</v>
-      </c>
       <c r="Q13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
       </c>
       <c r="C14" s="3">
         <v>43900</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1">
         <v>45240</v>
@@ -1863,39 +1863,39 @@
         <v>11</v>
       </c>
       <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" t="s">
         <v>62</v>
-      </c>
-      <c r="J14" t="s">
-        <v>19</v>
-      </c>
-      <c r="N14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="3">
         <v>44308</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1">
         <v>44148</v>
@@ -1907,39 +1907,39 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3">
         <v>45443</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="1">
         <v>43586</v>
@@ -1951,48 +1951,48 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K16" s="1">
         <v>45488</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>45299</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="1">
         <v>44628</v>
@@ -2004,45 +2004,45 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
         <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
       </c>
       <c r="C18" s="3">
         <v>45347</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1">
         <v>44307</v>
@@ -2054,48 +2054,48 @@
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K18" s="1">
         <v>45444</v>
       </c>
       <c r="L18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3">
         <v>45453</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1">
         <v>45061</v>
@@ -2107,45 +2107,45 @@
         <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3">
         <v>45618</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="1">
         <v>44048</v>
@@ -2157,45 +2157,45 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="1">
         <v>43660</v>
@@ -2207,45 +2207,45 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K21" s="1">
         <v>45366</v>
       </c>
       <c r="M21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3">
         <v>45364</v>
       </c>
       <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
         <v>30</v>
-      </c>
-      <c r="E22" t="s">
-        <v>31</v>
       </c>
       <c r="F22" s="1">
         <v>44939</v>
@@ -2257,39 +2257,39 @@
         <v>11</v>
       </c>
       <c r="I22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="3">
         <v>45399</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="1">
         <v>44113</v>
@@ -2301,36 +2301,36 @@
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="3">
         <v>45432</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" s="1">
         <v>43613</v>
@@ -2342,42 +2342,42 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K24" s="1">
         <v>45454</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3">
         <v>45597</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="1">
         <v>44755</v>
@@ -2389,42 +2389,42 @@
         <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="3">
         <v>45327</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F26" s="1">
         <v>44388</v>
@@ -2436,45 +2436,45 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K26" s="1">
         <v>45352</v>
       </c>
       <c r="L26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N26" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" t="s">
+        <v>20</v>
+      </c>
+      <c r="P26" t="s">
         <v>27</v>
       </c>
-      <c r="O26" t="s">
-        <v>21</v>
-      </c>
-      <c r="P26" t="s">
-        <v>28</v>
-      </c>
       <c r="Q26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="3">
         <v>45636</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" s="1">
         <v>44995</v>
@@ -2486,42 +2486,42 @@
         <v>11</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="3">
         <v>45411</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F28" s="1">
         <v>43044</v>
@@ -2533,42 +2533,42 @@
         <v>5</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" s="3">
         <v>45565</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F29" s="1">
         <v>43817</v>
@@ -2580,42 +2580,42 @@
         <v>3</v>
       </c>
       <c r="I29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K29" s="1">
         <v>45412</v>
       </c>
       <c r="L29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="3">
         <v>45323</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="1">
         <v>44633</v>
@@ -2627,45 +2627,45 @@
         <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="3">
         <v>45334</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F31" s="1">
         <v>44551</v>
@@ -2677,31 +2677,31 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K31" s="1">
         <v>45347</v>
       </c>
       <c r="L31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N31" t="s">
+        <v>26</v>
+      </c>
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+      <c r="P31" t="s">
         <v>27</v>
       </c>
-      <c r="O31" t="s">
-        <v>21</v>
-      </c>
-      <c r="P31" t="s">
-        <v>28</v>
-      </c>
       <c r="Q31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>